<commit_message>
criando comandos para criar a chave ssh
</commit_message>
<xml_diff>
--- a/git.xlsx
+++ b/git.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Informatica\GitGitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9322938-C120-4680-97B6-9C4617F174CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A0AB60-912B-498F-8EF3-575F5844C445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5F410918-A281-4185-B17F-F571408C196C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="108">
   <si>
     <t>git --version</t>
   </si>
@@ -337,6 +337,30 @@
   </si>
   <si>
     <t>envia as informações do repositorio para o servidor remoto</t>
+  </si>
+  <si>
+    <t>git pull</t>
+  </si>
+  <si>
+    <t>traz a ultima versão no servidor remoto</t>
+  </si>
+  <si>
+    <t>ssh-keygen</t>
+  </si>
+  <si>
+    <t>cd ~/.ssh/</t>
+  </si>
+  <si>
+    <t>start .</t>
+  </si>
+  <si>
+    <t>muda o nome dos arquivos</t>
+  </si>
+  <si>
+    <t>eval $(ssh-agent)</t>
+  </si>
+  <si>
+    <t>ssh-add ~/.ssh/nome_do_arquivo (não tem extenção)</t>
   </si>
 </sst>
 </file>
@@ -695,15 +719,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A257BFF9-B459-4C8C-BED9-7D00585C13BA}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.28515625" customWidth="1"/>
+    <col min="1" max="1" width="48.28515625" customWidth="1"/>
     <col min="2" max="2" width="97.140625" customWidth="1"/>
     <col min="3" max="3" width="85" customWidth="1"/>
   </cols>
@@ -1116,6 +1140,44 @@
         <v>99</v>
       </c>
     </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
fim do curso: comandos git
</commit_message>
<xml_diff>
--- a/git.xlsx
+++ b/git.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Informatica\GitGitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A144EF-8CC3-4E93-A105-62FA5F759D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622B0160-9580-4A65-8F1A-7737076BA8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5F410918-A281-4185-B17F-F571408C196C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="245">
   <si>
     <t>git --version</t>
   </si>
@@ -139,12 +139,6 @@
   </si>
   <si>
     <t>lista o penultimo commit e assim vai git log -3...-n</t>
-  </si>
-  <si>
-    <t>git log --oneline -1</t>
-  </si>
-  <si>
-    <t>lista o ultimo commit de forma resumida</t>
   </si>
   <si>
     <t>git log --patch</t>
@@ -571,6 +565,235 @@
   </si>
   <si>
     <t>todas as alterações feitas no arquivo expecifico são perdidas e volta as informações do ultimo commit (não podem estar na area de preparação)</t>
+  </si>
+  <si>
+    <t>git revert HEAD</t>
+  </si>
+  <si>
+    <t>cria um novo commit desfanzendo todas as alterações feitas no commit referente ao ponteiro HEAD</t>
+  </si>
+  <si>
+    <t>git revert HEAD --no-edit</t>
+  </si>
+  <si>
+    <t>reverte o que já tinha sido revertido (cria um novo commit)</t>
+  </si>
+  <si>
+    <t>apaga o ultimo commit</t>
+  </si>
+  <si>
+    <t>git reset --hard HEAD~1</t>
+  </si>
+  <si>
+    <t>git reset --hard HEAD~5</t>
+  </si>
+  <si>
+    <t>apaga os ultimos 5 commits (git reset --hard HEAD~1.......n)</t>
+  </si>
+  <si>
+    <t>git commit -a -m "Primeira Vesão"</t>
+  </si>
+  <si>
+    <t>salva as alterações no repostioria com a mesnsagem sem precisar de digitar "git add ."</t>
+  </si>
+  <si>
+    <t>git reset --mixed HEAD~1</t>
+  </si>
+  <si>
+    <t>git reset --soft HEAD~1</t>
+  </si>
+  <si>
+    <t>apaga o ultimo commit e não apaga as alterações feitas (fica na area modified)</t>
+  </si>
+  <si>
+    <t>apaga o ultimo commit e não apaga as alterações feitas (fica na area starged)</t>
+  </si>
+  <si>
+    <t>git push --force</t>
+  </si>
+  <si>
+    <t>atualiza o servidor sobescrevendo o que exite no remoto (o historico do repositorio remoto será perdio e substituido pelo local)</t>
+  </si>
+  <si>
+    <t>git push --force-with-lease</t>
+  </si>
+  <si>
+    <t>atualiza o servidor, vair subescrever a linha do tempo, mas desde que nenhuma alteração ser perdida durante o processo.</t>
+  </si>
+  <si>
+    <t>git rebase main</t>
+  </si>
+  <si>
+    <t>mescla a branch com main (no caso da main ter sido alterada e ter commits que a branch não tenha)</t>
+  </si>
+  <si>
+    <t>git rebase --abort</t>
+  </si>
+  <si>
+    <t>cancelar o rebase devido aos conflitos</t>
+  </si>
+  <si>
+    <t>git rebase --continue</t>
+  </si>
+  <si>
+    <t>após resolvido os conflitos emitir este comando para executar o rebase</t>
+  </si>
+  <si>
+    <t>git remote remove &lt;alias&gt;</t>
+  </si>
+  <si>
+    <t>remove o alias (caminho do servidor)</t>
+  </si>
+  <si>
+    <t>git pull --rebase</t>
+  </si>
+  <si>
+    <t>mescla o servidor remoto com main (no caso o servidor remoto ter sido alterada e ter commits que a branch não tenha)</t>
+  </si>
+  <si>
+    <t>git fetch &lt;alias_remoto&gt; &lt;branch_do_servidor&gt;</t>
+  </si>
+  <si>
+    <t>git branch -a</t>
+  </si>
+  <si>
+    <t>lista todas as branch inclusive as que foi baixada e que ainda não estaligada a sua main (não foi feito chechout na branch)</t>
+  </si>
+  <si>
+    <t>git rebase --interactive HEAD~3</t>
+  </si>
+  <si>
+    <t>Unir os três ultimos commits em um</t>
+  </si>
+  <si>
+    <t>git rebase --interactive HEAD~2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Unir os dois ultimos commits em um (o editor vair abrir a palavra </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>squash</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> na frente dos commits que vão ser fundidos menos no 1°)</t>
+    </r>
+  </si>
+  <si>
+    <t>git log --oneline -3</t>
+  </si>
+  <si>
+    <t>lista os três ultimo commit de forma resumida</t>
+  </si>
+  <si>
+    <t>git cherry-pick &lt;n°_do_commit_branch_desejada&gt;</t>
+  </si>
+  <si>
+    <t>faz um merge de um commite anterior da branch desejada ( você não quer mesclar com o commit autal da branch)</t>
+  </si>
+  <si>
+    <t>traz uma branch especifica para o servidor especifica do servidor.</t>
+  </si>
+  <si>
+    <t>git bisect good &lt;n°_do_commit&gt;</t>
+  </si>
+  <si>
+    <t>git bisect bad &lt;n°_do_commit&gt;</t>
+  </si>
+  <si>
+    <t>git bisect start</t>
+  </si>
+  <si>
+    <t>Faz uma busca binaria rasreando a modificação não desejada</t>
+  </si>
+  <si>
+    <t>git bisect reset</t>
+  </si>
+  <si>
+    <t>git fetch</t>
+  </si>
+  <si>
+    <t>git pull = git fetch + fet merge ( faço o git fetch para saber o que tem de diferente antes de mesclar)</t>
+  </si>
+  <si>
+    <t>mostras as branch que eu busquei no servidor (ainda não estão ligadas ao meu repositorio local)</t>
+  </si>
+  <si>
+    <t>git log &lt;alias_remoto&gt;/main --oneline</t>
+  </si>
+  <si>
+    <t>git diff &lt;alias_remoto&gt;/main</t>
+  </si>
+  <si>
+    <t>mostra as diferenças</t>
+  </si>
+  <si>
+    <t>git checkout  &lt;alias_remoto&gt;/main</t>
+  </si>
+  <si>
+    <t>git merge</t>
+  </si>
+  <si>
+    <t>git config --global alias.&lt;nome_do_alias&gt; &lt;comando&gt;</t>
+  </si>
+  <si>
+    <t>Exemplo: git config --global alias.s status (cria um apelido para o comando)</t>
+  </si>
+  <si>
+    <t>git config --global alias.&lt;nome_do_alias&gt; '&lt;comando&gt;'</t>
+  </si>
+  <si>
+    <t>colocar aspas simple se o comando tiver paramentros Ex.: git config --global alias.line 'log --oneline'</t>
+  </si>
+  <si>
+    <t>git config --global unset alias.&lt;nome_do_alias&gt;</t>
+  </si>
+  <si>
+    <t>apaga o apelido</t>
+  </si>
+  <si>
+    <t>git branch | grep "entre com nome parcial da branch"</t>
+  </si>
+  <si>
+    <t>Exemplo: git branch | grep ac -&gt; vai lista todas as branch que tem 'ac' em seu nome</t>
+  </si>
+  <si>
+    <t>git log --oneline | grep "entre com nome parcial da msn</t>
+  </si>
+  <si>
+    <t>Exemplo: git log --oneline | grep ac -&gt; vai lista todos os commits de tem uma mensagem tem 'ac' em sua composicao</t>
+  </si>
+  <si>
+    <t>sourcetree</t>
+  </si>
+  <si>
+    <t>gitkraken</t>
+  </si>
+  <si>
+    <t>ferramenta grafica para trabalhar com o git (windows e mac)</t>
+  </si>
+  <si>
+    <t>ferramenta grafica para trabalhar com o git (windows, mac e linux)</t>
+  </si>
+  <si>
+    <t>git GUI</t>
+  </si>
+  <si>
+    <t>gerramenta grafica que veem com o git</t>
   </si>
 </sst>
 </file>
@@ -608,7 +831,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -693,21 +916,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1022,16 +1284,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A257BFF9-B459-4C8C-BED9-7D00585C13BA}">
-  <dimension ref="A1:B98"/>
+  <dimension ref="A1:B136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A134" sqref="A134:B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="99" style="2" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="103.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1084,15 +1346,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
@@ -1156,654 +1418,944 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>184</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>65</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>40</v>
+        <v>211</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>212</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>177</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>88</v>
+        <v>200</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>89</v>
+        <v>201</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B52" s="4"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="B53" s="6"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="5"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+      <c r="B54" s="6"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B51" s="7"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
+      <c r="B55" s="6"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B52" s="7"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="B56" s="6"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B53" s="7"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B54" s="7"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B55" s="9"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="B57" s="8"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>63</v>
+        <v>130</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>139</v>
+        <v>61</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B94" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B95" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B96" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B98" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B99" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="B96" s="1" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B100" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>175</v>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="B118" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B119" s="10"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B120" s="10"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B121" s="11"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B122" s="9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B123" s="10" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B124" s="10"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="B125" s="10" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="B126" s="10"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B127" s="10"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="B128" s="11"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>